<commit_message>
micole finish dorm management module
</commit_message>
<xml_diff>
--- a/public/uploads/excel/warden (2).xlsx
+++ b/public/uploads/excel/warden (2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3373A68-62E4-49C6-88D2-CF25DA9D708D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2C7359-31A9-414C-A858-8DD0D11167D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,16 +43,16 @@
     <t>No. Tel Bimbit</t>
   </si>
   <si>
-    <t>warden 2</t>
-  </si>
-  <si>
-    <t>warden2@gmail.com</t>
-  </si>
-  <si>
-    <t>warden 3</t>
-  </si>
-  <si>
-    <t>warden3@gmail.com</t>
+    <t>warden 4</t>
+  </si>
+  <si>
+    <t>warden 5</t>
+  </si>
+  <si>
+    <t>warden4@gmail.com</t>
+  </si>
+  <si>
+    <t>warden5@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -427,30 +427,31 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C2">
-        <v>1012121213</v>
+        <v>109654782</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C3">
-        <v>109659743</v>
+        <v>123698699</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{2D453A2F-1EC3-42D5-9810-DA5E6C0D1B33}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{9D7CFA77-156E-423F-BBCE-FCB01C0DF0A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>